<commit_message>
Tweaks to serial HDF5 before moving onto parallel.
</commit_message>
<xml_diff>
--- a/LUMA/tools/RefinementGuide.xlsx
+++ b/LUMA/tools/RefinementGuide.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="84">
   <si>
     <t>Computational domain size according with L</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>% LUPTS</t>
+  </si>
+  <si>
+    <t>LUMA Refs</t>
+  </si>
+  <si>
+    <t>Object @</t>
   </si>
 </sst>
 </file>
@@ -579,7 +585,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -611,12 +617,19 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="110">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1136,13 +1149,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>105784</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>23309</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>437478</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>68132</xdr:rowOff>
@@ -1483,34 +1496,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1985,10 +1998,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:V40"/>
+  <dimension ref="A4:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2005,22 +2018,24 @@
     <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="8" customWidth="1"/>
+    <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>4</v>
       </c>
@@ -2031,48 +2046,55 @@
         <v>77</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14" t="s">
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="W8" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="X8" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="T8" s="14" t="s">
+      <c r="Y8" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="U8" s="14" t="s">
+      <c r="Z8" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="V8" s="14" t="s">
+      <c r="AA8" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="18">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>68</v>
@@ -2099,42 +2121,43 @@
       <c r="N9" s="18">
         <v>25</v>
       </c>
-      <c r="P9" t="s">
+      <c r="O9" s="24"/>
+      <c r="U9" t="s">
         <v>62</v>
       </c>
-      <c r="Q9">
+      <c r="V9">
         <f>F9*H9*C9^2</f>
-        <v>360000</v>
-      </c>
-      <c r="R9">
+        <v>250000</v>
+      </c>
+      <c r="W9">
         <f>C9^2*(F9*H9-F10*H10)</f>
-        <v>356544</v>
-      </c>
-      <c r="S9" s="16">
+        <v>247600</v>
+      </c>
+      <c r="X9" s="16">
         <f>(F9*H9-F10*H10)/(F9*H9)</f>
         <v>0.99039999999999995</v>
       </c>
-      <c r="T9" s="15">
-        <f>R9/R15</f>
+      <c r="Y9" s="15">
+        <f>W9/W15</f>
         <v>0.88051209103840677</v>
       </c>
-      <c r="U9">
-        <f>R9</f>
-        <v>356544</v>
-      </c>
-      <c r="V9" s="15">
-        <f>U9/$U$15</f>
+      <c r="Z9">
+        <f>W9</f>
+        <v>247600</v>
+      </c>
+      <c r="AA9" s="15">
+        <f>Z9/$Z$15</f>
         <v>0.5551569506726457</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="B10" t="s">
         <v>43</v>
       </c>
       <c r="C10">
         <f>C9*2</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -2164,42 +2187,58 @@
         <f>N9-(H10-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="26">
+        <f>L10*$C$9</f>
+        <v>190</v>
+      </c>
+      <c r="Q10" s="26">
+        <f>(L10+F10)*$C$9</f>
+        <v>270</v>
+      </c>
+      <c r="R10" s="26">
+        <f>N10*$C$9</f>
+        <v>240</v>
+      </c>
+      <c r="S10" s="26">
+        <f>(N10+H10)*$C$9</f>
+        <v>270</v>
+      </c>
+      <c r="U10" t="s">
         <v>63</v>
       </c>
-      <c r="Q10">
+      <c r="V10">
         <f>F10*H10*C10^2</f>
-        <v>13824</v>
-      </c>
-      <c r="R10">
+        <v>9600</v>
+      </c>
+      <c r="W10">
         <f>C10^2*(F10*H10-F11*H11)</f>
-        <v>9216</v>
-      </c>
-      <c r="S10" s="16">
+        <v>6400</v>
+      </c>
+      <c r="X10" s="16">
         <f>(F10*H10-F11*H11)/(F9*H9)</f>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="T10" s="15">
-        <f>R10/R15</f>
+      <c r="Y10" s="15">
+        <f>W10/W15</f>
         <v>2.2759601706970129E-2</v>
       </c>
-      <c r="U10">
-        <f>R10*2</f>
-        <v>18432</v>
-      </c>
-      <c r="V10" s="15">
-        <f t="shared" ref="V10:V12" si="0">U10/$U$15</f>
+      <c r="Z10">
+        <f>W10*2</f>
+        <v>12800</v>
+      </c>
+      <c r="AA10" s="15">
+        <f t="shared" ref="AA10:AA12" si="0">Z10/$Z$15</f>
         <v>2.8699551569506727E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>44</v>
       </c>
       <c r="C11">
         <f>C10*2</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
@@ -2228,42 +2267,58 @@
         <f>N9-(H11-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="26">
+        <f>(L11-L10)*$C$10</f>
+        <v>10</v>
+      </c>
+      <c r="Q11" s="26">
+        <f>(L11-L10+F11)*$C$10</f>
+        <v>90</v>
+      </c>
+      <c r="R11" s="26">
+        <f>(N11-N10)*$C$10</f>
+        <v>10</v>
+      </c>
+      <c r="S11" s="26">
+        <f>(N11-N10+H11)*$C$10</f>
+        <v>50</v>
+      </c>
+      <c r="U11" t="s">
         <v>64</v>
       </c>
-      <c r="Q11">
+      <c r="V11">
         <f>F11*H11*C11^2</f>
-        <v>18432</v>
-      </c>
-      <c r="R11">
+        <v>12800</v>
+      </c>
+      <c r="W11">
         <f>C11^2*(H11*F11-F12*H12)</f>
-        <v>11520</v>
-      </c>
-      <c r="S11" s="16">
+        <v>8000</v>
+      </c>
+      <c r="X11" s="16">
         <f>(F11*H11-F12*H12)/(F9*H9)</f>
         <v>2E-3</v>
       </c>
-      <c r="T11" s="15">
-        <f>R11/R15</f>
+      <c r="Y11" s="15">
+        <f>W11/W15</f>
         <v>2.8449502133712661E-2</v>
       </c>
-      <c r="U11">
-        <f>R11*4</f>
-        <v>46080</v>
-      </c>
-      <c r="V11" s="15">
+      <c r="Z11">
+        <f>W11*4</f>
+        <v>32000</v>
+      </c>
+      <c r="AA11" s="15">
         <f t="shared" si="0"/>
         <v>7.1748878923766815E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" t="s">
         <v>45</v>
       </c>
       <c r="C12">
         <f>C11*2</f>
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
@@ -2292,80 +2347,109 @@
         <f>N9-(H12-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="26">
+        <f>(L12-L11)*$C$11</f>
+        <v>10</v>
+      </c>
+      <c r="Q12" s="26">
+        <f>(L12-L11+F12)*$C$11</f>
+        <v>90</v>
+      </c>
+      <c r="R12" s="26">
+        <f>(N12-N11)*$C$11</f>
+        <v>10</v>
+      </c>
+      <c r="S12" s="26">
+        <f>(N12-N11+H12)*$C$11</f>
+        <v>70</v>
+      </c>
+      <c r="U12" t="s">
         <v>65</v>
       </c>
-      <c r="Q12">
+      <c r="V12">
         <f>F12*H12*C12^2</f>
-        <v>27648</v>
-      </c>
-      <c r="R12">
-        <f>Q12</f>
-        <v>27648</v>
-      </c>
-      <c r="S12" s="16">
+        <v>19200</v>
+      </c>
+      <c r="W12">
+        <f>V12</f>
+        <v>19200</v>
+      </c>
+      <c r="X12" s="16">
         <f>(F12*H12)/(F9*H9)</f>
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="T12" s="15">
-        <f>R12/R15</f>
+      <c r="Y12" s="15">
+        <f>W12/W15</f>
         <v>6.8278805120910391E-2</v>
       </c>
-      <c r="U12">
-        <f>R12*8</f>
-        <v>221184</v>
-      </c>
-      <c r="V12" s="15">
+      <c r="Z12">
+        <f>W12*8</f>
+        <v>153600</v>
+      </c>
+      <c r="AA12" s="15">
         <f t="shared" si="0"/>
         <v>0.34439461883408073</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
-      <c r="T13" s="15"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Y13" s="15"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>83</v>
+      </c>
+      <c r="P14" s="27">
+        <f>($F$12-1)/2 *$C$12</f>
+        <v>40</v>
+      </c>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
-      <c r="P15" t="s">
+      <c r="P15" s="27">
+        <f>($H$12-1)/2 *$C$12</f>
+        <v>20</v>
+      </c>
+      <c r="U15" t="s">
         <v>74</v>
       </c>
-      <c r="R15">
-        <f>SUM(R9:R12)</f>
-        <v>404928</v>
-      </c>
-      <c r="S15" s="17">
-        <f>SUM(S9:S12)</f>
+      <c r="W15">
+        <f>SUM(W9:W12)</f>
+        <v>281200</v>
+      </c>
+      <c r="X15" s="17">
+        <f>SUM(X9:X12)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="T15" s="17">
-        <f>SUM(T9:T12)</f>
+      <c r="Y15" s="17">
+        <f>SUM(Y9:Y12)</f>
         <v>1</v>
       </c>
-      <c r="U15">
-        <f>SUM(U9:U12)</f>
-        <v>642240</v>
-      </c>
-      <c r="V15" s="15">
-        <f>SUM(V9:V12)</f>
+      <c r="Z15">
+        <f>SUM(Z9:Z12)</f>
+        <v>446000</v>
+      </c>
+      <c r="AA15" s="15">
+        <f>SUM(AA9:AA12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>5</v>
       </c>
@@ -2376,48 +2460,55 @@
         <v>77</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="22" t="s">
+      <c r="K19" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14" t="s">
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="R19" s="14" t="s">
+      <c r="W19" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="S19" s="14" t="s">
+      <c r="X19" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="T19" s="14" t="s">
+      <c r="Y19" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="U19" s="14" t="s">
+      <c r="Z19" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="V19" s="14" t="s">
+      <c r="AA19" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
         <v>68</v>
@@ -2444,42 +2535,43 @@
       <c r="N20" s="18">
         <v>25</v>
       </c>
-      <c r="P20" t="s">
+      <c r="O20" s="24"/>
+      <c r="U20" t="s">
         <v>62</v>
       </c>
-      <c r="Q20">
+      <c r="V20">
         <f>F20*H20*C20^2</f>
-        <v>90000</v>
-      </c>
-      <c r="R20">
+        <v>62500</v>
+      </c>
+      <c r="W20">
         <f>C20^2*(F20*H20-F21*H21)</f>
-        <v>87696</v>
-      </c>
-      <c r="S20" s="16">
+        <v>60900</v>
+      </c>
+      <c r="X20" s="16">
         <f>(F20*H20-F21*H21)/(F20*H20)</f>
         <v>0.97440000000000004</v>
       </c>
-      <c r="T20" s="15">
-        <f>R20/R27</f>
+      <c r="Y20" s="15">
+        <f>W20/W27</f>
         <v>0.61827411167512691</v>
       </c>
-      <c r="U20">
-        <f>R20</f>
-        <v>87696</v>
-      </c>
-      <c r="V20" s="15">
-        <f>U20/$U$27</f>
+      <c r="Z20">
+        <f>W20</f>
+        <v>60900</v>
+      </c>
+      <c r="AA20" s="15">
+        <f>Z20/$Z$27</f>
         <v>0.13077088254240929</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" t="s">
         <v>43</v>
       </c>
       <c r="C21">
         <f>C20*2</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -2509,42 +2601,59 @@
         <f>N20-(H21-1)/2</f>
         <v>23.5</v>
       </c>
-      <c r="P21" t="s">
+      <c r="O21" s="25"/>
+      <c r="P21" s="26">
+        <f>L21*$C$20</f>
+        <v>92.5</v>
+      </c>
+      <c r="Q21" s="26">
+        <f>(L21+F21)*$C$20</f>
+        <v>172.5</v>
+      </c>
+      <c r="R21" s="26">
+        <f>N21*$C$20</f>
+        <v>117.5</v>
+      </c>
+      <c r="S21" s="26">
+        <f>(N21+H21)*$C$20</f>
+        <v>137.5</v>
+      </c>
+      <c r="U21" t="s">
         <v>63</v>
       </c>
-      <c r="Q21">
+      <c r="V21">
         <f>F21*H21*C21^2</f>
-        <v>9216</v>
-      </c>
-      <c r="R21">
+        <v>6400</v>
+      </c>
+      <c r="W21">
         <f>C21^2*(F21*H21-F22*H22)</f>
-        <v>5760</v>
-      </c>
-      <c r="S21" s="16">
+        <v>4000</v>
+      </c>
+      <c r="X21" s="16">
         <f>(F21*H21-F22*H22)/(F20*H20)</f>
         <v>1.6E-2</v>
       </c>
-      <c r="T21" s="15">
-        <f>R21/R27</f>
+      <c r="Y21" s="15">
+        <f>W21/W27</f>
         <v>4.060913705583756E-2</v>
       </c>
-      <c r="U21">
-        <f>R21*2</f>
-        <v>11520</v>
-      </c>
-      <c r="V21" s="15">
-        <f t="shared" ref="V21:V24" si="1">U21/$U$27</f>
+      <c r="Z21">
+        <f>W21*2</f>
+        <v>8000</v>
+      </c>
+      <c r="AA21" s="15">
+        <f t="shared" ref="AA21:AA24" si="1">Z21/$Z$27</f>
         <v>1.7178441056474127E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" t="s">
         <v>44</v>
       </c>
       <c r="C22">
         <f>C21*2</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
         <v>35</v>
@@ -2574,42 +2683,58 @@
         <f>N20-(H22-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22" s="26">
+        <f>(L22-L21)*$C$21</f>
+        <v>5</v>
+      </c>
+      <c r="Q22" s="26">
+        <f>(L22-L21+F22)*$C$21</f>
+        <v>85</v>
+      </c>
+      <c r="R22" s="26">
+        <f>(N22-N21)*$C$21</f>
+        <v>5</v>
+      </c>
+      <c r="S22" s="26">
+        <f>(N22-N21+H22)*$C$21</f>
+        <v>35</v>
+      </c>
+      <c r="U22" t="s">
         <v>64</v>
       </c>
-      <c r="Q22">
+      <c r="V22">
         <f>F22*H22*C22^2</f>
-        <v>13824</v>
-      </c>
-      <c r="R22">
+        <v>9600</v>
+      </c>
+      <c r="W22">
         <f>C22^2*(H22*F22-H23*F23)</f>
-        <v>9216</v>
-      </c>
-      <c r="S22" s="16">
+        <v>6400</v>
+      </c>
+      <c r="X22" s="16">
         <f>(F22*H22-F23*H23)/(F20*H20)</f>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="T22" s="15">
-        <f>R22/R27</f>
+      <c r="Y22" s="15">
+        <f>W22/W27</f>
         <v>6.4974619289340105E-2</v>
       </c>
-      <c r="U22">
-        <f>R22*4</f>
-        <v>36864</v>
-      </c>
-      <c r="V22" s="15">
+      <c r="Z22">
+        <f>W22*4</f>
+        <v>25600</v>
+      </c>
+      <c r="AA22" s="15">
         <f t="shared" si="1"/>
         <v>5.4971011380717201E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" t="s">
         <v>45</v>
       </c>
       <c r="C23">
         <f>C22*2</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
         <v>37</v>
@@ -2639,42 +2764,58 @@
         <f>N20-(H23-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="26">
+        <f>(L23-L22)*$C$22</f>
+        <v>10</v>
+      </c>
+      <c r="Q23" s="26">
+        <f>(L23-L22+F23)*$C$22</f>
+        <v>90</v>
+      </c>
+      <c r="R23" s="26">
+        <f>(N23-N22)*$C$22</f>
+        <v>10</v>
+      </c>
+      <c r="S23" s="26">
+        <f>(N23-N22+H23)*$C$22</f>
+        <v>50</v>
+      </c>
+      <c r="U23" t="s">
         <v>65</v>
       </c>
-      <c r="Q23">
+      <c r="V23">
         <f>F23*H23*C23^2</f>
-        <v>18432</v>
-      </c>
-      <c r="R23">
+        <v>12800</v>
+      </c>
+      <c r="W23">
         <f>C23^2*(H23*F23-H24*F24)</f>
-        <v>11520</v>
-      </c>
-      <c r="S23" s="16">
+        <v>8000</v>
+      </c>
+      <c r="X23" s="16">
         <f>(F23*H23-F24*H24)/(F20*H20)</f>
         <v>2E-3</v>
       </c>
-      <c r="T23" s="15">
-        <f>R23/R27</f>
+      <c r="Y23" s="15">
+        <f>W23/W27</f>
         <v>8.1218274111675121E-2</v>
       </c>
-      <c r="U23">
-        <f>R23*8</f>
-        <v>92160</v>
-      </c>
-      <c r="V23" s="15">
+      <c r="Z23">
+        <f>W23*8</f>
+        <v>64000</v>
+      </c>
+      <c r="AA23" s="15">
         <f t="shared" si="1"/>
         <v>0.13742752845179301</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" t="s">
         <v>46</v>
       </c>
       <c r="C24">
         <f>C23*2</f>
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
         <v>39</v>
@@ -2703,70 +2844,99 @@
         <f>N20-(H24-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="26">
+        <f>(L24-L23)*$C$23</f>
+        <v>10</v>
+      </c>
+      <c r="Q24" s="26">
+        <f>(L24-L23+F24)*$C$23</f>
+        <v>90</v>
+      </c>
+      <c r="R24" s="26">
+        <f>(N24-N23)*$C$23</f>
+        <v>10</v>
+      </c>
+      <c r="S24" s="26">
+        <f>(N24-N23+H24)*$C$23</f>
+        <v>70</v>
+      </c>
+      <c r="U24" t="s">
         <v>66</v>
       </c>
-      <c r="Q24">
+      <c r="V24">
         <f>F24*H24*C24^2</f>
-        <v>27648</v>
-      </c>
-      <c r="R24">
-        <f>Q24</f>
-        <v>27648</v>
-      </c>
-      <c r="S24" s="16">
+        <v>19200</v>
+      </c>
+      <c r="W24">
+        <f>V24</f>
+        <v>19200</v>
+      </c>
+      <c r="X24" s="16">
         <f>(F24*H24)/(F20*H20)</f>
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="T24" s="15">
-        <f>R24/R27</f>
+      <c r="Y24" s="15">
+        <f>W24/W27</f>
         <v>0.1949238578680203</v>
       </c>
-      <c r="U24">
-        <f>R24*16</f>
-        <v>442368</v>
-      </c>
-      <c r="V24" s="15">
+      <c r="Z24">
+        <f>W24*16</f>
+        <v>307200</v>
+      </c>
+      <c r="AA24" s="15">
         <f t="shared" si="1"/>
         <v>0.65965213656860644</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O26" t="s">
+        <v>83</v>
+      </c>
+      <c r="P26" s="27">
+        <f>($F$24-1)/2 *$C$24</f>
+        <v>40</v>
+      </c>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
-      <c r="P27" t="s">
+      <c r="P27" s="27">
+        <f>($H$24-1)/2 *$C$24</f>
+        <v>20</v>
+      </c>
+      <c r="U27" t="s">
         <v>74</v>
       </c>
-      <c r="R27">
-        <f>SUM(R20:R24)</f>
-        <v>141840</v>
-      </c>
-      <c r="S27" s="17">
-        <f>SUM(S20:S24)</f>
+      <c r="W27">
+        <f>SUM(W20:W24)</f>
+        <v>98500</v>
+      </c>
+      <c r="X27" s="17">
+        <f>SUM(X20:X24)</f>
         <v>1</v>
       </c>
-      <c r="T27" s="17">
-        <f>SUM(T20:T24)</f>
+      <c r="Y27" s="17">
+        <f>SUM(Y20:Y24)</f>
         <v>1</v>
       </c>
-      <c r="U27">
-        <f>SUM(U20:U24)</f>
-        <v>670608</v>
-      </c>
-      <c r="V27" s="15">
-        <f>SUM(V20:V24)</f>
+      <c r="Z27">
+        <f>SUM(Z20:Z24)</f>
+        <v>465700</v>
+      </c>
+      <c r="AA27" s="15">
+        <f>SUM(AA20:AA24)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>6</v>
       </c>
@@ -2791,33 +2961,40 @@
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
       <c r="N31" s="20"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14" t="s">
+      <c r="O31" s="21"/>
+      <c r="P31" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="R31" s="14" t="s">
+      <c r="W31" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="S31" s="14" t="s">
+      <c r="X31" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="T31" s="14" t="s">
+      <c r="Y31" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="U31" s="14" t="s">
+      <c r="Z31" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="V31" s="14" t="s">
+      <c r="AA31" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="18">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="E32" t="s">
         <v>68</v>
@@ -2844,41 +3021,42 @@
       <c r="N32" s="18">
         <v>25</v>
       </c>
-      <c r="P32" t="s">
+      <c r="O32" s="24"/>
+      <c r="U32" t="s">
         <v>62</v>
       </c>
-      <c r="Q32">
+      <c r="V32">
         <f>F32*H32*C32^2</f>
-        <v>22500</v>
-      </c>
-      <c r="R32">
+        <v>15625</v>
+      </c>
+      <c r="W32">
         <f>C32^2*(F32*H32-F33*H33)</f>
-        <v>21060</v>
-      </c>
-      <c r="S32" s="16">
+        <v>14625</v>
+      </c>
+      <c r="X32" s="16">
         <f>(F32*H32-F33*H33)/(F32*H32)</f>
         <v>0.93600000000000005</v>
       </c>
-      <c r="T32" s="15">
-        <f t="shared" ref="T32:T37" si="2">R32/$R$40</f>
+      <c r="Y32" s="15">
+        <f t="shared" ref="Y32:Y37" si="2">W32/$W$40</f>
         <v>0.26773455377574373</v>
       </c>
-      <c r="U32">
-        <f>R32</f>
-        <v>21060</v>
-      </c>
-      <c r="V32" s="15">
-        <f t="shared" ref="V32:V36" si="3">U32/$U$40</f>
+      <c r="Z32">
+        <f>W32</f>
+        <v>14625</v>
+      </c>
+      <c r="AA32" s="15">
+        <f t="shared" ref="AA32:AA36" si="3">Z32/$Z$40</f>
         <v>1.7641205030005127E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>43</v>
       </c>
       <c r="C33">
         <f>C32*2</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
         <v>33</v>
@@ -2908,41 +3086,57 @@
         <f>N32-(H33-1)/2</f>
         <v>23</v>
       </c>
-      <c r="P33" t="s">
+      <c r="P33" s="26">
+        <f>L33*$C$32</f>
+        <v>45</v>
+      </c>
+      <c r="Q33" s="26">
+        <f>(L33+F33)*$C$32</f>
+        <v>125</v>
+      </c>
+      <c r="R33" s="26">
+        <f>N33*$C$32</f>
+        <v>57.5</v>
+      </c>
+      <c r="S33" s="26">
+        <f>(N33+H33)*$C$32</f>
+        <v>70</v>
+      </c>
+      <c r="U33" t="s">
         <v>63</v>
       </c>
-      <c r="Q33">
+      <c r="V33">
         <f>F33*H33*C33^2</f>
-        <v>5760</v>
-      </c>
-      <c r="R33">
+        <v>4000</v>
+      </c>
+      <c r="W33">
         <f>C33^2*(F33*H33-F34*H34)</f>
-        <v>3456</v>
-      </c>
-      <c r="S33" s="16">
+        <v>2400</v>
+      </c>
+      <c r="X33" s="16">
         <f>(F33*H33-F34*H34)/(F32*H32)</f>
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="T33" s="15">
+      <c r="Y33" s="15">
         <f t="shared" si="2"/>
         <v>4.3935926773455376E-2</v>
       </c>
-      <c r="U33">
-        <f>R33*2</f>
-        <v>6912</v>
-      </c>
-      <c r="V33" s="15">
+      <c r="Z33">
+        <f>W33*2</f>
+        <v>4800</v>
+      </c>
+      <c r="AA33" s="15">
         <f t="shared" si="3"/>
         <v>5.7899339585657855E-3</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>44</v>
       </c>
       <c r="C34">
         <f>C33*2</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
         <v>35</v>
@@ -2972,41 +3166,57 @@
         <f>N32-(H34-1)/2</f>
         <v>23.5</v>
       </c>
-      <c r="P34" t="s">
+      <c r="P34" s="26">
+        <f>(L34-L33)*$C$33</f>
+        <v>2.5</v>
+      </c>
+      <c r="Q34" s="26">
+        <f>(L34-L33+F34)*$C$33</f>
+        <v>82.5</v>
+      </c>
+      <c r="R34" s="26">
+        <f>(N34-N33)*$C$33</f>
+        <v>2.5</v>
+      </c>
+      <c r="S34" s="26">
+        <f>(N34-N33+H34)*$C$33</f>
+        <v>22.5</v>
+      </c>
+      <c r="U34" t="s">
         <v>64</v>
       </c>
-      <c r="Q34">
+      <c r="V34">
         <f>F34*H34*C34^2</f>
-        <v>9216</v>
-      </c>
-      <c r="R34">
+        <v>6400</v>
+      </c>
+      <c r="W34">
         <f>C34^2*(F34*H34-F35*H35)</f>
-        <v>5760</v>
-      </c>
-      <c r="S34" s="16">
+        <v>4000</v>
+      </c>
+      <c r="X34" s="16">
         <f>(F34*H34-F35*H35)/(F32*H32)</f>
         <v>1.6E-2</v>
       </c>
-      <c r="T34" s="15">
+      <c r="Y34" s="15">
         <f t="shared" si="2"/>
         <v>7.3226544622425629E-2</v>
       </c>
-      <c r="U34">
-        <f>R34*4</f>
-        <v>23040</v>
-      </c>
-      <c r="V34" s="15">
+      <c r="Z34">
+        <f>W34*4</f>
+        <v>16000</v>
+      </c>
+      <c r="AA34" s="15">
         <f t="shared" si="3"/>
         <v>1.9299779861885951E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>45</v>
       </c>
       <c r="C35">
         <f>C34*2</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
         <v>37</v>
@@ -3036,41 +3246,57 @@
         <f>N32-(H35-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P35" s="26">
+        <f>(L35-L34)*$C$34</f>
+        <v>5</v>
+      </c>
+      <c r="Q35" s="26">
+        <f>(L35-L34+F35)*$C$34</f>
+        <v>85</v>
+      </c>
+      <c r="R35" s="26">
+        <f>(N35-N34)*$C$34</f>
+        <v>5</v>
+      </c>
+      <c r="S35" s="26">
+        <f>(N35-N34+H35)*$C$34</f>
+        <v>35</v>
+      </c>
+      <c r="U35" t="s">
         <v>65</v>
       </c>
-      <c r="Q35">
-        <f t="shared" ref="Q35:Q37" si="4">F35*H35*C35^2</f>
-        <v>13824</v>
-      </c>
-      <c r="R35">
+      <c r="V35">
+        <f t="shared" ref="V35:V37" si="4">F35*H35*C35^2</f>
+        <v>9600</v>
+      </c>
+      <c r="W35">
         <f>C35^2*(F35*H35-F36*H36)</f>
-        <v>9216</v>
-      </c>
-      <c r="S35" s="16">
+        <v>6400</v>
+      </c>
+      <c r="X35" s="16">
         <f>(F35*H35-F36*H36)/(F32*H32)</f>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="T35" s="15">
+      <c r="Y35" s="15">
         <f t="shared" si="2"/>
         <v>0.11716247139588101</v>
       </c>
-      <c r="U35">
-        <f>R35*8</f>
-        <v>73728</v>
-      </c>
-      <c r="V35" s="15">
+      <c r="Z35">
+        <f>W35*8</f>
+        <v>51200</v>
+      </c>
+      <c r="AA35" s="15">
         <f t="shared" si="3"/>
         <v>6.1759295558035041E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>46</v>
       </c>
       <c r="C36">
         <f>C35*2</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E36" t="s">
         <v>39</v>
@@ -3100,41 +3326,57 @@
         <f>N32-(H36-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P36" t="s">
+      <c r="P36" s="26">
+        <f>(L36-L35)*$C$35</f>
+        <v>10</v>
+      </c>
+      <c r="Q36" s="26">
+        <f>(L36-L35+F36)*$C$35</f>
+        <v>90</v>
+      </c>
+      <c r="R36" s="26">
+        <f>(N36-N35)*$C$35</f>
+        <v>10</v>
+      </c>
+      <c r="S36" s="26">
+        <f>(N36-N35+H36)*$C$35</f>
+        <v>50</v>
+      </c>
+      <c r="U36" t="s">
         <v>66</v>
       </c>
-      <c r="Q36">
+      <c r="V36">
         <f t="shared" si="4"/>
-        <v>18432</v>
-      </c>
-      <c r="R36">
+        <v>12800</v>
+      </c>
+      <c r="W36">
         <f>C36^2*(F36*H36-F37*H37)</f>
-        <v>11520</v>
-      </c>
-      <c r="S36" s="16">
+        <v>8000</v>
+      </c>
+      <c r="X36" s="16">
         <f>(F36*H36-F37*H37)/(F32*H32)</f>
         <v>2E-3</v>
       </c>
-      <c r="T36" s="15">
+      <c r="Y36" s="15">
         <f t="shared" si="2"/>
         <v>0.14645308924485126</v>
       </c>
-      <c r="U36">
-        <f>R36*16</f>
-        <v>184320</v>
-      </c>
-      <c r="V36" s="15">
+      <c r="Z36">
+        <f>W36*16</f>
+        <v>128000</v>
+      </c>
+      <c r="AA36" s="15">
         <f t="shared" si="3"/>
         <v>0.15439823889508761</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>47</v>
       </c>
       <c r="C37">
         <f>C36*2</f>
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E37" t="s">
         <v>41</v>
@@ -3163,56 +3405,87 @@
         <f>N32-(H37-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="26">
+        <f>(L37-L36)*$C$36</f>
+        <v>10</v>
+      </c>
+      <c r="Q37" s="26">
+        <f>(L37-L36+F37)*$C$36</f>
+        <v>90</v>
+      </c>
+      <c r="R37" s="26">
+        <f>(N37-N36)*$C$36</f>
+        <v>10</v>
+      </c>
+      <c r="S37" s="26">
+        <f>(N37-N36+H37)*$C$36</f>
+        <v>70</v>
+      </c>
+      <c r="U37" t="s">
         <v>67</v>
       </c>
-      <c r="Q37">
+      <c r="V37">
         <f t="shared" si="4"/>
-        <v>27648</v>
-      </c>
-      <c r="R37">
-        <f>Q37</f>
-        <v>27648</v>
-      </c>
-      <c r="S37" s="16">
+        <v>19200</v>
+      </c>
+      <c r="W37">
+        <f>V37</f>
+        <v>19200</v>
+      </c>
+      <c r="X37" s="16">
         <f>(F37*H37)/(F32*H32)</f>
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="T37" s="15">
+      <c r="Y37" s="15">
         <f t="shared" si="2"/>
         <v>0.35148741418764301</v>
       </c>
-      <c r="U37">
-        <f>R37*32</f>
-        <v>884736</v>
-      </c>
-      <c r="V37" s="15">
-        <f>U37/$U$40</f>
+      <c r="Z37">
+        <f>W37*32</f>
+        <v>614400</v>
+      </c>
+      <c r="AA37" s="15">
+        <f>Z37/$Z$40</f>
         <v>0.74111154669642054</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="P40" t="s">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="O39" t="s">
+        <v>83</v>
+      </c>
+      <c r="P39" s="27">
+        <f>($F$37-1)/2 *$C$37</f>
+        <v>40</v>
+      </c>
+      <c r="R39" s="27"/>
+      <c r="S39" s="27"/>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="P40" s="27">
+        <f>($H$37-1)/2 *$C$37</f>
+        <v>20</v>
+      </c>
+      <c r="U40" t="s">
         <v>74</v>
       </c>
-      <c r="R40">
-        <f>SUM(R32:R37)</f>
-        <v>78660</v>
-      </c>
-      <c r="S40" s="17">
-        <f>SUM(S32:S37)</f>
+      <c r="W40">
+        <f>SUM(W32:W37)</f>
+        <v>54625</v>
+      </c>
+      <c r="X40" s="17">
+        <f>SUM(X32:X37)</f>
         <v>1</v>
       </c>
-      <c r="T40" s="17">
-        <f>SUM(T32:T37)</f>
+      <c r="Y40" s="17">
+        <f>SUM(Y32:Y37)</f>
         <v>1</v>
       </c>
-      <c r="U40">
-        <f>SUM(U32:U37)</f>
-        <v>1193796</v>
-      </c>
-      <c r="V40" s="15">
-        <f>SUM(V32:V37)</f>
+      <c r="Z40">
+        <f>SUM(Z32:Z37)</f>
+        <v>829025</v>
+      </c>
+      <c r="AA40" s="15">
+        <f>SUM(AA32:AA37)</f>
         <v>1</v>
       </c>
     </row>
@@ -3224,8 +3497,8 @@
     <mergeCell ref="K19:N19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fix for HDF5 sub-grid in wall and new debugging options
</commit_message>
<xml_diff>
--- a/LUMA/tools/RefinementGuide.xlsx
+++ b/LUMA/tools/RefinementGuide.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="88">
   <si>
     <t>Computational domain size according with L</t>
   </si>
@@ -313,6 +313,18 @@
   </si>
   <si>
     <t>Object @</t>
+  </si>
+  <si>
+    <t>RefXstart</t>
+  </si>
+  <si>
+    <t>RefXend</t>
+  </si>
+  <si>
+    <t>RefYstart</t>
+  </si>
+  <si>
+    <t>RefYend</t>
   </si>
 </sst>
 </file>
@@ -585,7 +597,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -620,16 +632,19 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="110">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1075,8 +1090,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13022035" y="580036"/>
-          <a:ext cx="8446294" cy="6745143"/>
+          <a:off x="11748407" y="590921"/>
+          <a:ext cx="7491979" cy="8359858"/>
           <a:chOff x="11579678" y="607250"/>
           <a:chExt cx="7611723" cy="8604786"/>
         </a:xfrm>
@@ -1496,34 +1511,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2001,7 +2016,7 @@
   <dimension ref="A4:AA40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2019,7 +2034,10 @@
     <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="8" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" customWidth="1"/>
     <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
@@ -2046,27 +2064,27 @@
         <v>77</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
       <c r="O8" s="21"/>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
       <c r="V8" s="14" t="s">
@@ -2121,7 +2139,19 @@
       <c r="N9" s="18">
         <v>25</v>
       </c>
-      <c r="O9" s="24"/>
+      <c r="O9" s="22"/>
+      <c r="P9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>85</v>
+      </c>
+      <c r="R9" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" t="s">
+        <v>87</v>
+      </c>
       <c r="U9" t="s">
         <v>62</v>
       </c>
@@ -2187,19 +2217,19 @@
         <f>N9-(H10-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P10" s="26">
+      <c r="P10" s="24">
         <f>L10*$C$9</f>
         <v>190</v>
       </c>
-      <c r="Q10" s="26">
+      <c r="Q10" s="24">
         <f>(L10+F10)*$C$9</f>
         <v>270</v>
       </c>
-      <c r="R10" s="26">
+      <c r="R10" s="24">
         <f>N10*$C$9</f>
         <v>240</v>
       </c>
-      <c r="S10" s="26">
+      <c r="S10" s="24">
         <f>(N10+H10)*$C$9</f>
         <v>270</v>
       </c>
@@ -2267,19 +2297,19 @@
         <f>N9-(H11-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P11" s="26">
+      <c r="P11" s="24">
         <f>(L11-L10)*$C$10</f>
         <v>10</v>
       </c>
-      <c r="Q11" s="26">
+      <c r="Q11" s="24">
         <f>(L11-L10+F11)*$C$10</f>
         <v>90</v>
       </c>
-      <c r="R11" s="26">
+      <c r="R11" s="24">
         <f>(N11-N10)*$C$10</f>
         <v>10</v>
       </c>
-      <c r="S11" s="26">
+      <c r="S11" s="24">
         <f>(N11-N10+H11)*$C$10</f>
         <v>50</v>
       </c>
@@ -2347,19 +2377,19 @@
         <f>N9-(H12-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P12" s="26">
+      <c r="P12" s="24">
         <f>(L12-L11)*$C$11</f>
         <v>10</v>
       </c>
-      <c r="Q12" s="26">
+      <c r="Q12" s="24">
         <f>(L12-L11+F12)*$C$11</f>
         <v>90</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="24">
         <f>(N12-N11)*$C$11</f>
         <v>10</v>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="24">
         <f>(N12-N11+H12)*$C$11</f>
         <v>70</v>
       </c>
@@ -2400,19 +2430,19 @@
       <c r="O14" t="s">
         <v>83</v>
       </c>
-      <c r="P14" s="27">
+      <c r="P14" s="25">
         <f>($F$12-1)/2 *$C$12</f>
         <v>40</v>
       </c>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
+      <c r="Q14" s="25">
+        <f>($H$12-1)/2 *$C$12</f>
+        <v>20</v>
+      </c>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
-      <c r="P15" s="27">
-        <f>($H$12-1)/2 *$C$12</f>
-        <v>20</v>
-      </c>
       <c r="U15" t="s">
         <v>74</v>
       </c>
@@ -2460,27 +2490,27 @@
         <v>77</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="23" t="s">
+      <c r="K19" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
       <c r="O19" s="21"/>
-      <c r="P19" s="21" t="s">
+      <c r="P19" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
       <c r="V19" s="14" t="s">
@@ -2535,7 +2565,19 @@
       <c r="N20" s="18">
         <v>25</v>
       </c>
-      <c r="O20" s="24"/>
+      <c r="O20" s="22"/>
+      <c r="P20" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>85</v>
+      </c>
+      <c r="R20" t="s">
+        <v>86</v>
+      </c>
+      <c r="S20" t="s">
+        <v>87</v>
+      </c>
       <c r="U20" t="s">
         <v>62</v>
       </c>
@@ -2601,20 +2643,20 @@
         <f>N20-(H21-1)/2</f>
         <v>23.5</v>
       </c>
-      <c r="O21" s="25"/>
-      <c r="P21" s="26">
+      <c r="O21" s="23"/>
+      <c r="P21" s="24">
         <f>L21*$C$20</f>
         <v>92.5</v>
       </c>
-      <c r="Q21" s="26">
+      <c r="Q21" s="24">
         <f>(L21+F21)*$C$20</f>
         <v>172.5</v>
       </c>
-      <c r="R21" s="26">
+      <c r="R21" s="24">
         <f>N21*$C$20</f>
         <v>117.5</v>
       </c>
-      <c r="S21" s="26">
+      <c r="S21" s="24">
         <f>(N21+H21)*$C$20</f>
         <v>137.5</v>
       </c>
@@ -2683,19 +2725,19 @@
         <f>N20-(H22-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P22" s="26">
+      <c r="P22" s="24">
         <f>(L22-L21)*$C$21</f>
         <v>5</v>
       </c>
-      <c r="Q22" s="26">
+      <c r="Q22" s="24">
         <f>(L22-L21+F22)*$C$21</f>
         <v>85</v>
       </c>
-      <c r="R22" s="26">
+      <c r="R22" s="24">
         <f>(N22-N21)*$C$21</f>
         <v>5</v>
       </c>
-      <c r="S22" s="26">
+      <c r="S22" s="24">
         <f>(N22-N21+H22)*$C$21</f>
         <v>35</v>
       </c>
@@ -2764,19 +2806,19 @@
         <f>N20-(H23-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P23" s="26">
+      <c r="P23" s="24">
         <f>(L23-L22)*$C$22</f>
         <v>10</v>
       </c>
-      <c r="Q23" s="26">
+      <c r="Q23" s="24">
         <f>(L23-L22+F23)*$C$22</f>
         <v>90</v>
       </c>
-      <c r="R23" s="26">
+      <c r="R23" s="24">
         <f>(N23-N22)*$C$22</f>
         <v>10</v>
       </c>
-      <c r="S23" s="26">
+      <c r="S23" s="24">
         <f>(N23-N22+H23)*$C$22</f>
         <v>50</v>
       </c>
@@ -2844,19 +2886,19 @@
         <f>N20-(H24-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P24" s="26">
+      <c r="P24" s="24">
         <f>(L24-L23)*$C$23</f>
         <v>10</v>
       </c>
-      <c r="Q24" s="26">
+      <c r="Q24" s="24">
         <f>(L24-L23+F24)*$C$23</f>
         <v>90</v>
       </c>
-      <c r="R24" s="26">
+      <c r="R24" s="24">
         <f>(N24-N23)*$C$23</f>
         <v>10</v>
       </c>
-      <c r="S24" s="26">
+      <c r="S24" s="24">
         <f>(N24-N23+H24)*$C$23</f>
         <v>70</v>
       </c>
@@ -2896,19 +2938,19 @@
       <c r="O26" t="s">
         <v>83</v>
       </c>
-      <c r="P26" s="27">
+      <c r="P26" s="25">
         <f>($F$24-1)/2 *$C$24</f>
         <v>40</v>
       </c>
-      <c r="R26" s="27"/>
-      <c r="S26" s="27"/>
+      <c r="Q26" s="25">
+        <f>($H$24-1)/2 *$C$24</f>
+        <v>20</v>
+      </c>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
-      <c r="P27" s="27">
-        <f>($H$24-1)/2 *$C$24</f>
-        <v>20</v>
-      </c>
       <c r="U27" t="s">
         <v>74</v>
       </c>
@@ -2962,12 +3004,12 @@
       <c r="M31" s="20"/>
       <c r="N31" s="20"/>
       <c r="O31" s="21"/>
-      <c r="P31" s="21" t="s">
+      <c r="P31" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="28"/>
       <c r="T31" s="14"/>
       <c r="U31" s="14"/>
       <c r="V31" s="14" t="s">
@@ -3021,7 +3063,19 @@
       <c r="N32" s="18">
         <v>25</v>
       </c>
-      <c r="O32" s="24"/>
+      <c r="O32" s="22"/>
+      <c r="P32" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>85</v>
+      </c>
+      <c r="R32" t="s">
+        <v>86</v>
+      </c>
+      <c r="S32" t="s">
+        <v>87</v>
+      </c>
       <c r="U32" t="s">
         <v>62</v>
       </c>
@@ -3086,19 +3140,19 @@
         <f>N32-(H33-1)/2</f>
         <v>23</v>
       </c>
-      <c r="P33" s="26">
+      <c r="P33" s="24">
         <f>L33*$C$32</f>
         <v>45</v>
       </c>
-      <c r="Q33" s="26">
+      <c r="Q33" s="24">
         <f>(L33+F33)*$C$32</f>
         <v>125</v>
       </c>
-      <c r="R33" s="26">
+      <c r="R33" s="24">
         <f>N33*$C$32</f>
         <v>57.5</v>
       </c>
-      <c r="S33" s="26">
+      <c r="S33" s="24">
         <f>(N33+H33)*$C$32</f>
         <v>70</v>
       </c>
@@ -3166,19 +3220,19 @@
         <f>N32-(H34-1)/2</f>
         <v>23.5</v>
       </c>
-      <c r="P34" s="26">
+      <c r="P34" s="24">
         <f>(L34-L33)*$C$33</f>
         <v>2.5</v>
       </c>
-      <c r="Q34" s="26">
+      <c r="Q34" s="24">
         <f>(L34-L33+F34)*$C$33</f>
         <v>82.5</v>
       </c>
-      <c r="R34" s="26">
+      <c r="R34" s="24">
         <f>(N34-N33)*$C$33</f>
         <v>2.5</v>
       </c>
-      <c r="S34" s="26">
+      <c r="S34" s="24">
         <f>(N34-N33+H34)*$C$33</f>
         <v>22.5</v>
       </c>
@@ -3246,19 +3300,19 @@
         <f>N32-(H35-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P35" s="26">
+      <c r="P35" s="24">
         <f>(L35-L34)*$C$34</f>
         <v>5</v>
       </c>
-      <c r="Q35" s="26">
+      <c r="Q35" s="24">
         <f>(L35-L34+F35)*$C$34</f>
         <v>85</v>
       </c>
-      <c r="R35" s="26">
+      <c r="R35" s="24">
         <f>(N35-N34)*$C$34</f>
         <v>5</v>
       </c>
-      <c r="S35" s="26">
+      <c r="S35" s="24">
         <f>(N35-N34+H35)*$C$34</f>
         <v>35</v>
       </c>
@@ -3326,19 +3380,19 @@
         <f>N32-(H36-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P36" s="26">
+      <c r="P36" s="24">
         <f>(L36-L35)*$C$35</f>
         <v>10</v>
       </c>
-      <c r="Q36" s="26">
+      <c r="Q36" s="24">
         <f>(L36-L35+F36)*$C$35</f>
         <v>90</v>
       </c>
-      <c r="R36" s="26">
+      <c r="R36" s="24">
         <f>(N36-N35)*$C$35</f>
         <v>10</v>
       </c>
-      <c r="S36" s="26">
+      <c r="S36" s="24">
         <f>(N36-N35+H36)*$C$35</f>
         <v>50</v>
       </c>
@@ -3405,19 +3459,19 @@
         <f>N32-(H37-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P37" s="26">
+      <c r="P37" s="24">
         <f>(L37-L36)*$C$36</f>
         <v>10</v>
       </c>
-      <c r="Q37" s="26">
+      <c r="Q37" s="24">
         <f>(L37-L36+F37)*$C$36</f>
         <v>90</v>
       </c>
-      <c r="R37" s="26">
+      <c r="R37" s="24">
         <f>(N37-N36)*$C$36</f>
         <v>10</v>
       </c>
-      <c r="S37" s="26">
+      <c r="S37" s="24">
         <f>(N37-N36+H37)*$C$36</f>
         <v>70</v>
       </c>
@@ -3453,18 +3507,18 @@
       <c r="O39" t="s">
         <v>83</v>
       </c>
-      <c r="P39" s="27">
+      <c r="P39" s="25">
         <f>($F$37-1)/2 *$C$37</f>
         <v>40</v>
       </c>
-      <c r="R39" s="27"/>
-      <c r="S39" s="27"/>
-    </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="P40" s="27">
+      <c r="Q39" s="25">
         <f>($H$37-1)/2 *$C$37</f>
         <v>20</v>
       </c>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
       <c r="U40" t="s">
         <v>74</v>
       </c>
@@ -3490,11 +3544,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="P31:S31"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="E8:I8"/>
     <mergeCell ref="E19:I19"/>
     <mergeCell ref="K19:N19"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="P19:S19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to latest alpha, incorporated force calculator into OM
</commit_message>
<xml_diff>
--- a/LUMA/tools/RefinementGuide.xlsx
+++ b/LUMA/tools/RefinementGuide.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="88">
   <si>
     <t>Computational domain size according with L</t>
   </si>
@@ -313,6 +313,18 @@
   </si>
   <si>
     <t>Object @</t>
+  </si>
+  <si>
+    <t>RefXstart</t>
+  </si>
+  <si>
+    <t>RefXend</t>
+  </si>
+  <si>
+    <t>RefYstart</t>
+  </si>
+  <si>
+    <t>RefYend</t>
   </si>
 </sst>
 </file>
@@ -585,7 +597,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -620,16 +632,19 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="110">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1075,8 +1090,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13022035" y="580036"/>
-          <a:ext cx="8446294" cy="6745143"/>
+          <a:off x="11748407" y="590921"/>
+          <a:ext cx="7491979" cy="8359858"/>
           <a:chOff x="11579678" y="607250"/>
           <a:chExt cx="7611723" cy="8604786"/>
         </a:xfrm>
@@ -1496,34 +1511,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2001,7 +2016,7 @@
   <dimension ref="A4:AA40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2019,7 +2034,10 @@
     <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" customWidth="1"/>
     <col min="15" max="15" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="8" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" customWidth="1"/>
     <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
@@ -2046,27 +2064,27 @@
         <v>77</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
       <c r="O8" s="21"/>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
       <c r="T8" s="14"/>
       <c r="U8" s="14"/>
       <c r="V8" s="14" t="s">
@@ -2121,7 +2139,19 @@
       <c r="N9" s="18">
         <v>25</v>
       </c>
-      <c r="O9" s="24"/>
+      <c r="O9" s="22"/>
+      <c r="P9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>85</v>
+      </c>
+      <c r="R9" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" t="s">
+        <v>87</v>
+      </c>
       <c r="U9" t="s">
         <v>62</v>
       </c>
@@ -2187,19 +2217,19 @@
         <f>N9-(H10-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P10" s="26">
+      <c r="P10" s="24">
         <f>L10*$C$9</f>
         <v>190</v>
       </c>
-      <c r="Q10" s="26">
+      <c r="Q10" s="24">
         <f>(L10+F10)*$C$9</f>
         <v>270</v>
       </c>
-      <c r="R10" s="26">
+      <c r="R10" s="24">
         <f>N10*$C$9</f>
         <v>240</v>
       </c>
-      <c r="S10" s="26">
+      <c r="S10" s="24">
         <f>(N10+H10)*$C$9</f>
         <v>270</v>
       </c>
@@ -2267,19 +2297,19 @@
         <f>N9-(H11-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P11" s="26">
+      <c r="P11" s="24">
         <f>(L11-L10)*$C$10</f>
         <v>10</v>
       </c>
-      <c r="Q11" s="26">
+      <c r="Q11" s="24">
         <f>(L11-L10+F11)*$C$10</f>
         <v>90</v>
       </c>
-      <c r="R11" s="26">
+      <c r="R11" s="24">
         <f>(N11-N10)*$C$10</f>
         <v>10</v>
       </c>
-      <c r="S11" s="26">
+      <c r="S11" s="24">
         <f>(N11-N10+H11)*$C$10</f>
         <v>50</v>
       </c>
@@ -2347,19 +2377,19 @@
         <f>N9-(H12-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P12" s="26">
+      <c r="P12" s="24">
         <f>(L12-L11)*$C$11</f>
         <v>10</v>
       </c>
-      <c r="Q12" s="26">
+      <c r="Q12" s="24">
         <f>(L12-L11+F12)*$C$11</f>
         <v>90</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="24">
         <f>(N12-N11)*$C$11</f>
         <v>10</v>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="24">
         <f>(N12-N11+H12)*$C$11</f>
         <v>70</v>
       </c>
@@ -2400,19 +2430,19 @@
       <c r="O14" t="s">
         <v>83</v>
       </c>
-      <c r="P14" s="27">
+      <c r="P14" s="25">
         <f>($F$12-1)/2 *$C$12</f>
         <v>40</v>
       </c>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
+      <c r="Q14" s="25">
+        <f>($H$12-1)/2 *$C$12</f>
+        <v>20</v>
+      </c>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
-      <c r="P15" s="27">
-        <f>($H$12-1)/2 *$C$12</f>
-        <v>20</v>
-      </c>
       <c r="U15" t="s">
         <v>74</v>
       </c>
@@ -2460,27 +2490,27 @@
         <v>77</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="23" t="s">
+      <c r="K19" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
       <c r="O19" s="21"/>
-      <c r="P19" s="21" t="s">
+      <c r="P19" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
       <c r="V19" s="14" t="s">
@@ -2535,7 +2565,19 @@
       <c r="N20" s="18">
         <v>25</v>
       </c>
-      <c r="O20" s="24"/>
+      <c r="O20" s="22"/>
+      <c r="P20" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>85</v>
+      </c>
+      <c r="R20" t="s">
+        <v>86</v>
+      </c>
+      <c r="S20" t="s">
+        <v>87</v>
+      </c>
       <c r="U20" t="s">
         <v>62</v>
       </c>
@@ -2601,20 +2643,20 @@
         <f>N20-(H21-1)/2</f>
         <v>23.5</v>
       </c>
-      <c r="O21" s="25"/>
-      <c r="P21" s="26">
+      <c r="O21" s="23"/>
+      <c r="P21" s="24">
         <f>L21*$C$20</f>
         <v>92.5</v>
       </c>
-      <c r="Q21" s="26">
+      <c r="Q21" s="24">
         <f>(L21+F21)*$C$20</f>
         <v>172.5</v>
       </c>
-      <c r="R21" s="26">
+      <c r="R21" s="24">
         <f>N21*$C$20</f>
         <v>117.5</v>
       </c>
-      <c r="S21" s="26">
+      <c r="S21" s="24">
         <f>(N21+H21)*$C$20</f>
         <v>137.5</v>
       </c>
@@ -2683,19 +2725,19 @@
         <f>N20-(H22-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P22" s="26">
+      <c r="P22" s="24">
         <f>(L22-L21)*$C$21</f>
         <v>5</v>
       </c>
-      <c r="Q22" s="26">
+      <c r="Q22" s="24">
         <f>(L22-L21+F22)*$C$21</f>
         <v>85</v>
       </c>
-      <c r="R22" s="26">
+      <c r="R22" s="24">
         <f>(N22-N21)*$C$21</f>
         <v>5</v>
       </c>
-      <c r="S22" s="26">
+      <c r="S22" s="24">
         <f>(N22-N21+H22)*$C$21</f>
         <v>35</v>
       </c>
@@ -2764,19 +2806,19 @@
         <f>N20-(H23-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P23" s="26">
+      <c r="P23" s="24">
         <f>(L23-L22)*$C$22</f>
         <v>10</v>
       </c>
-      <c r="Q23" s="26">
+      <c r="Q23" s="24">
         <f>(L23-L22+F23)*$C$22</f>
         <v>90</v>
       </c>
-      <c r="R23" s="26">
+      <c r="R23" s="24">
         <f>(N23-N22)*$C$22</f>
         <v>10</v>
       </c>
-      <c r="S23" s="26">
+      <c r="S23" s="24">
         <f>(N23-N22+H23)*$C$22</f>
         <v>50</v>
       </c>
@@ -2844,19 +2886,19 @@
         <f>N20-(H24-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P24" s="26">
+      <c r="P24" s="24">
         <f>(L24-L23)*$C$23</f>
         <v>10</v>
       </c>
-      <c r="Q24" s="26">
+      <c r="Q24" s="24">
         <f>(L24-L23+F24)*$C$23</f>
         <v>90</v>
       </c>
-      <c r="R24" s="26">
+      <c r="R24" s="24">
         <f>(N24-N23)*$C$23</f>
         <v>10</v>
       </c>
-      <c r="S24" s="26">
+      <c r="S24" s="24">
         <f>(N24-N23+H24)*$C$23</f>
         <v>70</v>
       </c>
@@ -2896,19 +2938,19 @@
       <c r="O26" t="s">
         <v>83</v>
       </c>
-      <c r="P26" s="27">
+      <c r="P26" s="25">
         <f>($F$24-1)/2 *$C$24</f>
         <v>40</v>
       </c>
-      <c r="R26" s="27"/>
-      <c r="S26" s="27"/>
+      <c r="Q26" s="25">
+        <f>($H$24-1)/2 *$C$24</f>
+        <v>20</v>
+      </c>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
-      <c r="P27" s="27">
-        <f>($H$24-1)/2 *$C$24</f>
-        <v>20</v>
-      </c>
       <c r="U27" t="s">
         <v>74</v>
       </c>
@@ -2962,12 +3004,12 @@
       <c r="M31" s="20"/>
       <c r="N31" s="20"/>
       <c r="O31" s="21"/>
-      <c r="P31" s="21" t="s">
+      <c r="P31" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="28"/>
       <c r="T31" s="14"/>
       <c r="U31" s="14"/>
       <c r="V31" s="14" t="s">
@@ -3021,7 +3063,19 @@
       <c r="N32" s="18">
         <v>25</v>
       </c>
-      <c r="O32" s="24"/>
+      <c r="O32" s="22"/>
+      <c r="P32" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>85</v>
+      </c>
+      <c r="R32" t="s">
+        <v>86</v>
+      </c>
+      <c r="S32" t="s">
+        <v>87</v>
+      </c>
       <c r="U32" t="s">
         <v>62</v>
       </c>
@@ -3086,19 +3140,19 @@
         <f>N32-(H33-1)/2</f>
         <v>23</v>
       </c>
-      <c r="P33" s="26">
+      <c r="P33" s="24">
         <f>L33*$C$32</f>
         <v>45</v>
       </c>
-      <c r="Q33" s="26">
+      <c r="Q33" s="24">
         <f>(L33+F33)*$C$32</f>
         <v>125</v>
       </c>
-      <c r="R33" s="26">
+      <c r="R33" s="24">
         <f>N33*$C$32</f>
         <v>57.5</v>
       </c>
-      <c r="S33" s="26">
+      <c r="S33" s="24">
         <f>(N33+H33)*$C$32</f>
         <v>70</v>
       </c>
@@ -3166,19 +3220,19 @@
         <f>N32-(H34-1)/2</f>
         <v>23.5</v>
       </c>
-      <c r="P34" s="26">
+      <c r="P34" s="24">
         <f>(L34-L33)*$C$33</f>
         <v>2.5</v>
       </c>
-      <c r="Q34" s="26">
+      <c r="Q34" s="24">
         <f>(L34-L33+F34)*$C$33</f>
         <v>82.5</v>
       </c>
-      <c r="R34" s="26">
+      <c r="R34" s="24">
         <f>(N34-N33)*$C$33</f>
         <v>2.5</v>
       </c>
-      <c r="S34" s="26">
+      <c r="S34" s="24">
         <f>(N34-N33+H34)*$C$33</f>
         <v>22.5</v>
       </c>
@@ -3246,19 +3300,19 @@
         <f>N32-(H35-1)/2</f>
         <v>24</v>
       </c>
-      <c r="P35" s="26">
+      <c r="P35" s="24">
         <f>(L35-L34)*$C$34</f>
         <v>5</v>
       </c>
-      <c r="Q35" s="26">
+      <c r="Q35" s="24">
         <f>(L35-L34+F35)*$C$34</f>
         <v>85</v>
       </c>
-      <c r="R35" s="26">
+      <c r="R35" s="24">
         <f>(N35-N34)*$C$34</f>
         <v>5</v>
       </c>
-      <c r="S35" s="26">
+      <c r="S35" s="24">
         <f>(N35-N34+H35)*$C$34</f>
         <v>35</v>
       </c>
@@ -3326,19 +3380,19 @@
         <f>N32-(H36-1)/2</f>
         <v>24.5</v>
       </c>
-      <c r="P36" s="26">
+      <c r="P36" s="24">
         <f>(L36-L35)*$C$35</f>
         <v>10</v>
       </c>
-      <c r="Q36" s="26">
+      <c r="Q36" s="24">
         <f>(L36-L35+F36)*$C$35</f>
         <v>90</v>
       </c>
-      <c r="R36" s="26">
+      <c r="R36" s="24">
         <f>(N36-N35)*$C$35</f>
         <v>10</v>
       </c>
-      <c r="S36" s="26">
+      <c r="S36" s="24">
         <f>(N36-N35+H36)*$C$35</f>
         <v>50</v>
       </c>
@@ -3405,19 +3459,19 @@
         <f>N32-(H37-1)/2</f>
         <v>24.75</v>
       </c>
-      <c r="P37" s="26">
+      <c r="P37" s="24">
         <f>(L37-L36)*$C$36</f>
         <v>10</v>
       </c>
-      <c r="Q37" s="26">
+      <c r="Q37" s="24">
         <f>(L37-L36+F37)*$C$36</f>
         <v>90</v>
       </c>
-      <c r="R37" s="26">
+      <c r="R37" s="24">
         <f>(N37-N36)*$C$36</f>
         <v>10</v>
       </c>
-      <c r="S37" s="26">
+      <c r="S37" s="24">
         <f>(N37-N36+H37)*$C$36</f>
         <v>70</v>
       </c>
@@ -3453,18 +3507,18 @@
       <c r="O39" t="s">
         <v>83</v>
       </c>
-      <c r="P39" s="27">
+      <c r="P39" s="25">
         <f>($F$37-1)/2 *$C$37</f>
         <v>40</v>
       </c>
-      <c r="R39" s="27"/>
-      <c r="S39" s="27"/>
-    </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="P40" s="27">
+      <c r="Q39" s="25">
         <f>($H$37-1)/2 *$C$37</f>
         <v>20</v>
       </c>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
       <c r="U40" t="s">
         <v>74</v>
       </c>
@@ -3490,11 +3544,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="P31:S31"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="E8:I8"/>
     <mergeCell ref="E19:I19"/>
     <mergeCell ref="K19:N19"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="P19:S19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>